<commit_message>
Complete search time analysis
Use RANDOMIZED to compare linear and complex bounded sort.
</commit_message>
<xml_diff>
--- a/dev-topics-codingexams/dev-topics-liveramp-bitsearch/analysis/Performance.xlsx
+++ b/dev-topics-codingexams/dev-topics-liveramp-bitsearch/analysis/Performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="128" windowWidth="22290" windowHeight="9218" activeTab="4"/>
+    <workbookView xWindow="300" yWindow="128" windowWidth="22290" windowHeight="9218"/>
   </bookViews>
   <sheets>
     <sheet name="Rand" sheetId="2" r:id="rId1"/>
@@ -343,7 +343,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>LoadTM!$B$3</c:f>
+              <c:f>LoadTM!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -354,7 +354,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>LoadTM!$A$4:$A$9</c:f>
+              <c:f>LoadTM!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -381,7 +381,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>LoadTM!$B$4:$B$9</c:f>
+              <c:f>LoadTM!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -413,7 +413,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>LoadTM!$C$3</c:f>
+              <c:f>LoadTM!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -424,7 +424,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>LoadTM!$A$4:$A$9</c:f>
+              <c:f>LoadTM!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -451,7 +451,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>LoadTM!$C$4:$C$9</c:f>
+              <c:f>LoadTM!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -483,7 +483,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>LoadTM!$D$3</c:f>
+              <c:f>LoadTM!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -494,7 +494,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>LoadTM!$A$4:$A$9</c:f>
+              <c:f>LoadTM!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -521,7 +521,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>LoadTM!$D$4:$D$9</c:f>
+              <c:f>LoadTM!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -556,11 +556,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="56653312"/>
-        <c:axId val="56655232"/>
+        <c:axId val="137201536"/>
+        <c:axId val="137207808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56653312"/>
+        <c:axId val="137201536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000000"/>
@@ -600,12 +600,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56655232"/>
+        <c:crossAx val="137207808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56655232"/>
+        <c:axId val="137207808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="550"/>
@@ -624,7 +624,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1200"/>
-                  <a:t>Timer in NS</a:t>
+                  <a:t>Time in NS</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US"/>
@@ -640,7 +640,330 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56653312"/>
+        <c:crossAx val="137201536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" baseline="0"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Population</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Search Time - Randomized</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.24876843005314098"/>
+          <c:y val="1.3574092712095198E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.384177142903645E-2"/>
+          <c:y val="4.4891493826429589E-2"/>
+          <c:w val="0.75635316108331574"/>
+          <c:h val="0.83424150928502361"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SearchTM!$H$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>uBS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SearchTM!$F$8:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>139000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>695000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1390000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2780000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3475000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4865000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SearchTM!$H$8:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SearchTM!$I$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>uSS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SearchTM!$F$8:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>139000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>695000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1390000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2780000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3475000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4865000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SearchTM!$I$8:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="66441600"/>
+        <c:axId val="66443520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="66441600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5000000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>IP</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> Access and Counts Population Size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>	</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66443520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="66443520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Time in NS</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>	</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66441600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -678,19 +1001,56 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>21430</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>538162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>637382</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1008,7 +1368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1332,11 +1694,11 @@
         <v>14</v>
       </c>
       <c r="M10" s="12">
-        <f t="shared" ref="M5:M68" si="0">ROUND(AVERAGE(F10:F15),0)</f>
+        <f t="shared" ref="M10:M64" si="0">ROUND(AVERAGE(F10:F15),0)</f>
         <v>23167</v>
       </c>
       <c r="N10" s="11">
-        <f t="shared" ref="N5:N68" si="1">ROUND(AVERAGE(J10:J15),2)</f>
+        <f t="shared" ref="N10:N64" si="1">ROUND(AVERAGE(J10:J15),2)</f>
         <v>0.17</v>
       </c>
     </row>
@@ -3612,11 +3974,11 @@
         <v>14</v>
       </c>
       <c r="M70" s="12">
-        <f t="shared" ref="M69:M75" si="2">ROUND(AVERAGE(F70:F75),0)</f>
+        <f t="shared" ref="M70" si="2">ROUND(AVERAGE(F70:F75),0)</f>
         <v>810833</v>
       </c>
       <c r="N70" s="11">
-        <f t="shared" ref="N69:N75" si="3">ROUND(AVERAGE(J70:J75),2)</f>
+        <f t="shared" ref="N70" si="3">ROUND(AVERAGE(J70:J75),2)</f>
         <v>11</v>
       </c>
     </row>
@@ -3815,7 +4177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6183,7 +6545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -8548,11 +8910,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I132"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -8571,235 +8931,238 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="9">
+        <f>Rand!E4</f>
+        <v>139000</v>
+      </c>
+      <c r="B3" s="7">
+        <f>Rand!H4</f>
+        <v>82</v>
+      </c>
+      <c r="C3" s="7">
+        <f>Rand!H10</f>
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <f>NotRand!H10</f>
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F8" si="0">C3-D3</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="10">
+        <f>F3/D3</f>
+        <v>0.25</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H8" si="1">B3-D3</f>
+        <v>74</v>
+      </c>
+      <c r="I3" s="10">
+        <f t="shared" ref="I3:I8" si="2">H3/D3</f>
+        <v>9.25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="9">
-        <f>Rand!E4</f>
-        <v>139000</v>
+        <f>Rand!E16</f>
+        <v>695000</v>
       </c>
       <c r="B4" s="7">
-        <f>Rand!H4</f>
-        <v>82</v>
+        <f>Rand!H16</f>
+        <v>81</v>
       </c>
       <c r="C4" s="7">
-        <f>Rand!H10</f>
-        <v>10</v>
+        <f>Rand!H22</f>
+        <v>34</v>
       </c>
       <c r="D4">
-        <f>NotRand!H10</f>
-        <v>8</v>
+        <f>NotRand!H22</f>
+        <v>17</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F9" si="0">C4-D4</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="G4" s="10">
-        <f>F4/D4</f>
-        <v>0.25</v>
+        <f t="shared" ref="G4:G8" si="3">F4/D4</f>
+        <v>1</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H9" si="1">B4-D4</f>
-        <v>74</v>
+        <f t="shared" si="1"/>
+        <v>64</v>
       </c>
       <c r="I4" s="10">
-        <f t="shared" ref="I4:I9" si="2">H4/D4</f>
-        <v>9.25</v>
+        <f t="shared" si="2"/>
+        <v>3.7647058823529411</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="9">
-        <f>Rand!E16</f>
-        <v>695000</v>
+        <f>Rand!E28</f>
+        <v>1390000</v>
       </c>
       <c r="B5" s="7">
-        <f>Rand!H16</f>
-        <v>81</v>
+        <f>Rand!H28</f>
+        <v>122</v>
       </c>
       <c r="C5" s="7">
-        <f>Rand!H22</f>
-        <v>34</v>
+        <f>Rand!H34</f>
+        <v>74</v>
       </c>
       <c r="D5">
-        <f>NotRand!H22</f>
-        <v>17</v>
+        <f>NotRand!H34</f>
+        <v>28</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="G5" s="10">
-        <f t="shared" ref="G5:G9" si="3">F5/D5</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>1.6428571428571428</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="I5" s="10">
         <f t="shared" si="2"/>
-        <v>3.7647058823529411</v>
+        <v>3.3571428571428572</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="9">
-        <f>Rand!E28</f>
-        <v>1390000</v>
+        <f>Rand!E40</f>
+        <v>2780000</v>
       </c>
       <c r="B6" s="7">
-        <f>Rand!H28</f>
-        <v>122</v>
+        <f>Rand!H40</f>
+        <v>150</v>
       </c>
       <c r="C6" s="7">
-        <f>Rand!H34</f>
-        <v>74</v>
+        <f>Rand!H46</f>
+        <v>504</v>
       </c>
       <c r="D6">
-        <f>NotRand!H34</f>
-        <v>28</v>
+        <f>NotRand!H46</f>
+        <v>376</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="G6" s="10">
         <f t="shared" si="3"/>
-        <v>1.6428571428571428</v>
+        <v>0.34042553191489361</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>94</v>
+        <v>-226</v>
       </c>
       <c r="I6" s="10">
         <f t="shared" si="2"/>
-        <v>3.3571428571428572</v>
+        <v>-0.60106382978723405</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="9">
-        <f>Rand!E40</f>
-        <v>2780000</v>
+        <f>Rand!E52</f>
+        <v>3475000</v>
       </c>
       <c r="B7" s="7">
-        <f>Rand!H40</f>
-        <v>150</v>
+        <f>Rand!H52</f>
+        <v>171</v>
       </c>
       <c r="C7" s="7">
-        <f>Rand!H46</f>
-        <v>504</v>
+        <f>Rand!H58</f>
+        <v>249</v>
       </c>
       <c r="D7">
-        <f>NotRand!H46</f>
-        <v>376</v>
+        <f>NotRand!H58</f>
+        <v>68</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>128</v>
+        <v>181</v>
       </c>
       <c r="G7" s="10">
         <f t="shared" si="3"/>
-        <v>0.34042553191489361</v>
+        <v>2.6617647058823528</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>-226</v>
+        <v>103</v>
       </c>
       <c r="I7" s="10">
         <f t="shared" si="2"/>
-        <v>-0.60106382978723405</v>
+        <v>1.5147058823529411</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="9">
-        <f>Rand!E52</f>
-        <v>3475000</v>
+        <f>Rand!E64</f>
+        <v>4865000</v>
       </c>
       <c r="B8" s="7">
-        <f>Rand!H52</f>
-        <v>171</v>
+        <f>Rand!H64</f>
+        <v>276</v>
       </c>
       <c r="C8" s="7">
-        <f>Rand!H58</f>
-        <v>249</v>
+        <f>Rand!H70</f>
+        <v>369</v>
       </c>
       <c r="D8">
-        <f>NotRand!H58</f>
-        <v>68</v>
+        <f>NotRand!H70</f>
+        <v>87</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>181</v>
+        <v>282</v>
       </c>
       <c r="G8" s="10">
         <f t="shared" si="3"/>
-        <v>2.6617647058823528</v>
+        <v>3.2413793103448274</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="I8" s="10">
         <f t="shared" si="2"/>
-        <v>1.5147058823529411</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="9">
-        <f>Rand!E64</f>
-        <v>4865000</v>
-      </c>
-      <c r="B9" s="7">
-        <f>Rand!H64</f>
-        <v>276</v>
-      </c>
-      <c r="C9" s="7">
-        <f>Rand!H70</f>
-        <v>369</v>
-      </c>
-      <c r="D9">
-        <f>NotRand!H70</f>
-        <v>87</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>282</v>
-      </c>
-      <c r="G9" s="10">
-        <f t="shared" si="3"/>
-        <v>3.2413793103448274</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>189</v>
-      </c>
-      <c r="I9" s="10">
-        <f t="shared" si="2"/>
         <v>2.1724137931034484</v>
       </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B11" s="5"/>
@@ -8813,8 +9176,8 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B15" s="5"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" s="5"/>
@@ -8828,8 +9191,8 @@
     <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B21" s="5"/>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B23" s="5"/>
@@ -8843,8 +9206,8 @@
     <row r="26" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B27" s="5"/>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B29" s="5"/>
@@ -8858,8 +9221,8 @@
     <row r="32" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B32" s="5"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B33" s="5"/>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" s="5"/>
@@ -8873,8 +9236,8 @@
     <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" s="5"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B39" s="5"/>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="5"/>
@@ -8882,8 +9245,8 @@
     <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" s="5"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B45" s="5"/>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B47" s="5"/>
@@ -8897,8 +9260,8 @@
     <row r="50" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B50" s="5"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B51" s="5"/>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B53" s="5"/>
@@ -8912,8 +9275,8 @@
     <row r="56" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B56" s="5"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B57" s="5"/>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B59" s="5"/>
@@ -8927,8 +9290,8 @@
     <row r="62" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B62" s="5"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B63" s="5"/>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B65" s="5"/>
@@ -8942,8 +9305,8 @@
     <row r="68" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B68" s="5"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B69" s="5"/>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B71" s="5"/>
@@ -9127,9 +9490,6 @@
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B131" s="5"/>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B132" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9141,8 +9501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="F6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9151,7 +9511,7 @@
     <col min="2" max="2" width="4.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.73046875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="5.19921875" bestFit="1" customWidth="1"/>
   </cols>
@@ -9253,7 +9613,7 @@
         <v>1.17</v>
       </c>
       <c r="E8" s="17"/>
-      <c r="F8" s="12">
+      <c r="F8" s="9">
         <f>A8</f>
         <v>139000</v>
       </c>
@@ -9287,7 +9647,7 @@
         <f>Rand!N10</f>
         <v>0.17</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="9">
         <f>A10</f>
         <v>695000</v>
       </c>
@@ -9321,7 +9681,7 @@
         <f>Rand!N16</f>
         <v>2.5</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="9">
         <f>A12</f>
         <v>1390000</v>
       </c>
@@ -9355,7 +9715,7 @@
         <f>Rand!N22</f>
         <v>1.5</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="9">
         <f>A14</f>
         <v>2780000</v>
       </c>
@@ -9389,7 +9749,7 @@
         <f>Rand!N28</f>
         <v>4.33</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="9">
         <f>A16</f>
         <v>3475000</v>
       </c>
@@ -9423,7 +9783,7 @@
         <f>Rand!N34</f>
         <v>3.17</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="9">
         <f>A18</f>
         <v>4865000</v>
       </c>
@@ -9866,5 +10226,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>